<commit_message>
Excel Changes in Index and View Page
</commit_message>
<xml_diff>
--- a/resources/assets/uploadandtemplates/templates/gensen_TEMP.xlsx
+++ b/resources/assets/uploadandtemplates/templates/gensen_TEMP.xlsx
@@ -7,66 +7,14 @@
     <workbookView xWindow="270" yWindow="585" windowWidth="27495" windowHeight="11025"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Gensen Employee" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
-  <si>
-    <t>First</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <r>
-      <t>L</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>ast</t>
-    </r>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <r>
-      <t>f</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>irst kana</t>
-    </r>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <r>
-      <t>L</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>ast kana</t>
-    </r>
-    <phoneticPr fontId="3"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <r>
       <t>D</t>
@@ -213,22 +161,6 @@
   </si>
   <si>
     <r>
-      <t>i</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>nsurance</t>
-    </r>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <r>
       <t>E</t>
     </r>
     <r>
@@ -241,6 +173,18 @@
       </rPr>
       <t>mp no</t>
     </r>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Name</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Kana Name</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Insurance</t>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -302,16 +246,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -322,10 +266,19 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="distributed" vertical="center"/>
     </xf>
@@ -335,13 +288,10 @@
     <xf numFmtId="57" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -657,91 +607,87 @@
   </cols>
   <sheetData>
     <row r="6" spans="2:7">
-      <c r="B6" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="5"/>
+      <c r="B6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="3"/>
     </row>
     <row r="9" spans="2:7">
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="2:7">
+      <c r="B10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="6"/>
+    </row>
+    <row r="11" spans="2:7" ht="37.5" customHeight="1">
+      <c r="B11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+    </row>
+    <row r="13" spans="2:7">
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="2:7">
+      <c r="B14" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="2:7">
+      <c r="B15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="2:7">
+      <c r="B16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="18" spans="2:4">
+      <c r="B18" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="2:7">
-      <c r="B10" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="2:7" ht="37.5" customHeight="1">
-      <c r="B11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-    </row>
-    <row r="13" spans="2:7">
-      <c r="C13" s="4"/>
-    </row>
-    <row r="14" spans="2:7">
-      <c r="B14" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7">
-      <c r="B15" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-    </row>
-    <row r="16" spans="2:7">
-      <c r="B16" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-    </row>
-    <row r="18" spans="2:4">
-      <c r="B18" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="5" t="s">
+      <c r="D18" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="5" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="19" spans="2:4">
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>

</xml_diff>